<commit_message>
Committed the modified file
</commit_message>
<xml_diff>
--- a/Controller_ONECONFIGFY21Test014.xlsx
+++ b/Controller_ONECONFIGFY21Test014.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\USM_Data\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9E2484-755B-45C7-971A-136526E18A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B14ABF-DFD8-41FD-8F57-4BEADCF98187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="11676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,10 +89,10 @@
     <t>Incognito</t>
   </si>
   <si>
-    <t>180</t>
-  </si>
-  <si>
-    <t>ScriptedFlow_UserManagementScript_PrePROD_62bd5233.xlsx</t>
+    <t>ScriptedFlow_POManagementScript_PrePROD_50bde6f4.xlsx</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.6640625" defaultRowHeight="14.4"/>
@@ -539,13 +539,13 @@
         <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L2" s="4"/>
     </row>

</xml_diff>